<commit_message>
Arbeidsmodaliteit en StamItems delen hetzelfde history mechanisme
</commit_message>
<xml_diff>
--- a/NVWA DTV/Referentielijsten.xlsx
+++ b/NVWA DTV/Referentielijsten.xlsx
@@ -4,57 +4,26 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4920" windowWidth="11448" windowHeight="4944" activeTab="1"/>
+    <workbookView xWindow="5136" yWindow="5964" windowWidth="11448" windowHeight="4944"/>
   </bookViews>
   <sheets>
-    <sheet name="Mutation" sheetId="1" r:id="rId1"/>
-    <sheet name="StamItem" sheetId="2" r:id="rId2"/>
-    <sheet name="Variable" sheetId="3" r:id="rId3"/>
+    <sheet name="StamItem" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="104">
-  <si>
-    <t>Mutation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
   <si>
     <t>Referentielijst</t>
   </si>
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
     <t>Wetsartikel</t>
   </si>
   <si>
-    <t>[Mutation]</t>
-  </si>
-  <si>
-    <t>[Variable]</t>
-  </si>
-  <si>
-    <t>deleted</t>
-  </si>
-  <si>
-    <t>mutGrond</t>
-  </si>
-  <si>
-    <t>mutNaam</t>
-  </si>
-  <si>
-    <t>pred</t>
-  </si>
-  <si>
     <t>refLijst</t>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t>var</t>
   </si>
   <si>
     <t>varGrond</t>
@@ -679,559 +648,472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
-      <c r="A2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="E15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="E17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="E18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>54</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B26" t="s">
         <v>55</v>
       </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>56</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="E22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>60</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
         <v>61</v>
       </c>
-      <c r="E24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D29" t="s">
         <v>63</v>
       </c>
-      <c r="E25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>64</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
         <v>65</v>
       </c>
-      <c r="E26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
-      <c r="E27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
         <v>71</v>
       </c>
-      <c r="C29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
         <v>74</v>
       </c>
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>76</v>
       </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
         <v>77</v>
       </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>79</v>
       </c>
-      <c r="E31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" t="s">
         <v>80</v>
       </c>
-      <c r="B32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>82</v>
       </c>
-      <c r="E32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
         <v>83</v>
       </c>
-      <c r="B33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>85</v>
       </c>
-      <c r="E33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
         <v>86</v>
       </c>
-      <c r="B34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>88</v>
       </c>
-      <c r="E34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" t="s">
         <v>89</v>
       </c>
-      <c r="B35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" t="s">
-        <v>97</v>
-      </c>
-      <c r="E37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
+      <c r="D38" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adapt to changing Ampersand compiler
</commit_message>
<xml_diff>
--- a/NVWA DTV/Referentielijsten.xlsx
+++ b/NVWA DTV/Referentielijsten.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1608" yWindow="2028" windowWidth="11448" windowHeight="4944"/>
+    <workbookView xWindow="1605" yWindow="2025" windowWidth="11445" windowHeight="4950"/>
   </bookViews>
   <sheets>
     <sheet name="StamItem" sheetId="2" r:id="rId1"/>
@@ -239,15 +239,9 @@
     <t>VariableName</t>
   </si>
   <si>
-    <t xml:space="preserve">Afbouwregeling inconvenienten          </t>
-  </si>
-  <si>
     <t>BBRA artikel 18, Arbeidsvoorwaarden NVWA</t>
   </si>
   <si>
-    <t>Afbouwregeling ploegendienst        </t>
-  </si>
-  <si>
     <t>BBRA art 17</t>
   </si>
   <si>
@@ -279,13 +273,19 @@
   </si>
   <si>
     <t>var35</t>
+  </si>
+  <si>
+    <t>Afbouwregeling inconvenienten</t>
+  </si>
+  <si>
+    <t>Afbouwregeling ploegendienst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -427,6 +427,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -461,6 +462,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -636,22 +638,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A36"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -665,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
@@ -679,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -690,7 +692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -698,24 +700,24 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -723,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -737,13 +739,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -751,13 +753,13 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -765,13 +767,13 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -779,13 +781,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -793,13 +795,13 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -807,13 +809,13 @@
         <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -821,13 +823,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -835,13 +837,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -849,13 +851,13 @@
         <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -863,13 +865,13 @@
         <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -877,13 +879,13 @@
         <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -891,13 +893,13 @@
         <v>37</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -905,13 +907,13 @@
         <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -919,13 +921,13 @@
         <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -933,13 +935,13 @@
         <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -947,13 +949,13 @@
         <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -961,13 +963,13 @@
         <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -975,13 +977,13 @@
         <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -989,13 +991,13 @@
         <v>51</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1003,13 +1005,13 @@
         <v>53</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1017,13 +1019,13 @@
         <v>55</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1031,13 +1033,13 @@
         <v>57</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1045,41 +1047,41 @@
         <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
       <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
       </c>
       <c r="D30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1087,13 +1089,13 @@
         <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1101,49 +1103,49 @@
         <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
         <v>61</v>

</xml_diff>